<commit_message>
Cambios a la BD en tabla uaprendizaje y p_ua, se elimino la clavessh
</commit_message>
<xml_diff>
--- a/documents/BITACORA_CAMBIOS_BD.xlsx
+++ b/documents/BITACORA_CAMBIOS_BD.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="114">
   <si>
     <t>planestudiodesc</t>
   </si>
@@ -341,6 +341,33 @@
   </si>
   <si>
     <t>Campo "semestre" agregado a la tabla carga (Registro 60)</t>
+  </si>
+  <si>
+    <t>UAPRENDIZAJE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se elimino el campo carácter y la llave foranea fk_uaprendizaje_caracter1 </t>
+  </si>
+  <si>
+    <t>Se elimino el campo semestre_sug</t>
+  </si>
+  <si>
+    <t>Se cambio por requerimiento de usuario</t>
+  </si>
+  <si>
+    <t>P_UA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se AGREGO el campo carácter y la llave foranea fk_uaprendizaje_caracter1 </t>
+  </si>
+  <si>
+    <t>Se AGREGO el campo semestre_sug</t>
+  </si>
+  <si>
+    <t>Ver registro 69</t>
+  </si>
+  <si>
+    <t>Ver registro 70</t>
   </si>
 </sst>
 </file>
@@ -803,12 +830,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1245" topLeftCell="A58" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+      <selection pane="bottomLeft" activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1721,7 @@
         <v>41961</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>96</v>
       </c>
@@ -1708,7 +1735,7 @@
         <v>41961</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>96</v>
       </c>
@@ -1722,7 +1749,7 @@
         <v>41961</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>101</v>
       </c>
@@ -1736,7 +1763,7 @@
         <v>41961</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>101</v>
       </c>
@@ -1745,6 +1772,68 @@
       </c>
       <c r="C68" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C69" t="s">
+        <v>106</v>
+      </c>
+      <c r="D69" s="2">
+        <v>41948</v>
+      </c>
+      <c r="G69" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" s="2">
+        <v>41948</v>
+      </c>
+      <c r="G70" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C71" t="s">
+        <v>110</v>
+      </c>
+      <c r="G71" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72" t="s">
+        <v>111</v>
+      </c>
+      <c r="G72" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios a Plan de Estudios full (faltan detalles), se actualizo script base de datos y se documentaron mas cambios a la BD
</commit_message>
<xml_diff>
--- a/documents/BITACORA_CAMBIOS_BD.xlsx
+++ b/documents/BITACORA_CAMBIOS_BD.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t>planestudiodesc</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>Ver registro 70</t>
+  </si>
+  <si>
+    <t>Se modificaron lo triggers de la bitacora quitando los campos semestre_sug y carácter</t>
+  </si>
+  <si>
+    <t>Se modificaron lo triggers de la bitacora añadiendo los campos semestre_sug y carácter</t>
   </si>
 </sst>
 </file>
@@ -830,12 +836,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1245" topLeftCell="A58" activePane="bottomLeft"/>
+      <pane ySplit="1245" topLeftCell="A64" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="G73" sqref="G73"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,6 +1842,34 @@
         <v>113</v>
       </c>
     </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" t="s">
+        <v>114</v>
+      </c>
+      <c r="D73" s="2">
+        <v>41948</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" t="s">
+        <v>115</v>
+      </c>
+      <c r="D74" s="2">
+        <v>41949</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A39:I39"/>

</xml_diff>